<commit_message>
Início do Exame Especial de Python2
</commit_message>
<xml_diff>
--- a/PosGraduacao/Desenvolvimento/Python/ArmazenamentoEProcessamentoMassivoEDistribuidoDeDados/Aula9/Exercicio.xlsx
+++ b/PosGraduacao/Desenvolvimento/Python/ArmazenamentoEProcessamentoMassivoEDistribuidoDeDados/Aula9/Exercicio.xlsx
@@ -28,34 +28,34 @@
     <t>Prova</t>
   </si>
   <si>
-    <t>Lorena da Costa</t>
-  </si>
-  <si>
-    <t>Lívia Farias</t>
-  </si>
-  <si>
-    <t>Otávio Carvalho</t>
-  </si>
-  <si>
-    <t>Raquel Correia</t>
-  </si>
-  <si>
-    <t>Sr. João Lucas Gomes</t>
-  </si>
-  <si>
-    <t>Alice Peixoto</t>
-  </si>
-  <si>
-    <t>Caio Viana</t>
-  </si>
-  <si>
-    <t>Daniela Rodrigues</t>
-  </si>
-  <si>
-    <t>Mariane Cunha</t>
-  </si>
-  <si>
-    <t>Maria Pires</t>
+    <t>Juliana da Mata</t>
+  </si>
+  <si>
+    <t>Sr. Gustavo Henrique da Cunha</t>
+  </si>
+  <si>
+    <t>Lucas Freitas</t>
+  </si>
+  <si>
+    <t>Dra. Helena da Conceição</t>
+  </si>
+  <si>
+    <t>Sr. Heitor Lima</t>
+  </si>
+  <si>
+    <t>Sr. Marcos Vinicius da Cruz</t>
+  </si>
+  <si>
+    <t>Rebeca Campos</t>
+  </si>
+  <si>
+    <t>Elisa Gomes</t>
+  </si>
+  <si>
+    <t>Emanuella Cardoso</t>
+  </si>
+  <si>
+    <t>Elisa da Cunha</t>
   </si>
 </sst>
 </file>
@@ -441,10 +441,10 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -455,10 +455,10 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -469,10 +469,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -483,10 +483,10 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -497,10 +497,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>95</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -511,10 +511,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>70</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -525,10 +525,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>45</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -539,10 +539,10 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -553,10 +553,10 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>90</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -567,10 +567,10 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>